<commit_message>
second commit 25-9-23 - Finish the user's login route and generate users collection on mongoDB
</commit_message>
<xml_diff>
--- a/Data base structure.xlsx
+++ b/Data base structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\NodeJS-Project\NodeJS-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\NodeJS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A4E81B-CEE1-407F-80A3-93C420A99C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A415B-E421-497C-ACBC-14CE1B7D7E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="970" activeTab="3" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="2" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
   <sheets>
     <sheet name="משימות" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="139">
   <si>
     <t>נושא</t>
   </si>
@@ -18169,12 +18169,198 @@
       <t>, required: true },</t>
     </r>
   </si>
+  <si>
+    <t>npm install express-session cookie-parser</t>
+  </si>
+  <si>
+    <t>npm i axios</t>
+  </si>
+  <si>
+    <t>Try the latest stable version of npm</t>
+  </si>
+  <si>
+    <t>Big Problem</t>
+  </si>
+  <si>
+    <t>Fix it</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Error:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot find module 'timers/promises'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Require stack:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\@npmcli\agent\lib\util.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\@npmcli\agent\lib\index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\make-fetch-happen\lib\remote.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\make-fetch-happen\lib\cache\entry.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\make-fetch-happen\lib\cache\index.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\make-fetch-happen\lib\fetch.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\make-fetch-happen\lib\index.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\npm-registry-fetch\lib\index.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\lib\utils\replace-info.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\lib\utils\error-message.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\lib\utils\exit-handler.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\lib\cli-entry.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\lib\cli.js
+- C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\bin\npm-cli.js
+    at Function.Module._resolveFilename (internal/modules/cjs/loader.js:880:15)
+    at Function.Module._load (internal/modules/cjs/loader.js:725:27)
+    at Module.require (internal/modules/cjs/loader.js:952:19)
+    at require (internal/modules/cjs/helpers.js:88:18)
+    at Object.&lt;anonymous&gt; (C:\Users\basheer\AppData\Roaming\npm\node_modules\npm\node_modules\@npmcli\agent\lib\util.js:3:16)
+    at Module._compile (internal/modules/cjs/loader.js:1063:30)
+    at Object.Module._extensions..js (internal/modules/cjs/loader.js:1092:10)
+    at Module.load (internal/modules/cjs/loader.js:928:32)
+    at Function.Module._load (internal/modules/cjs/loader.js:769:14)
+    at Module.require (internal/modules/cjs/loader.js:952:19) {
+  code: 'MODULE_NOT_FOUND',
+  requireStack: [
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\@npmcli\\agent\\lib\\util.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\@npmcli\\agent\\lib\\index.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\make-fetch-happen\\lib\\cache\\entry.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\make-fetch-happen\\lib\\cache\\index.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\make-fetch-happen\\lib\\fetch.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\make-fetch-happen\\lib\\index.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\node_modules\\npm-registry-fetch\\lib\\index.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\lib\\utils\\replace-info.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\lib\\utils\\error-message.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\lib\\utils\\exit-handler.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\lib\\cli-entry.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\lib\\cli.js',
+    'C:\\Users\\basheer\\AppData\\Roaming\\npm\\node_modules\\npm\\bin\\npm-cli.js'
+  ]
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>npm -v</t>
+  </si>
+  <si>
+    <t>Cammands</t>
+  </si>
+  <si>
+    <t>See what version of npm you're running</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upgrade to the latest version of npm </t>
+  </si>
+  <si>
+    <t>npm install -g npm@latest</t>
+  </si>
+  <si>
+    <t>By default, npm is installed alongside node in</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\nodejs</t>
+  </si>
+  <si>
+    <t>Option 3: Navigate to %ProgramFiles%\nodejs\node_modules\npm and copy the npmrcfile to another folder or the desktop. Then open cmd.exe as an administrator and run the following commands:</t>
+  </si>
+  <si>
+    <t>cd %ProgramFiles%\nodejs
+npm install npm@latest</t>
+  </si>
+  <si>
+    <t>Link to website</t>
+  </si>
+  <si>
+    <t>https://docs.npmjs.com/try-the-latest-stable-version-of-npm</t>
+  </si>
+  <si>
+    <t>npm i jsonfile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18292,8 +18478,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -18324,8 +18580,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -18512,11 +18792,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -18587,24 +18984,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -18632,8 +19011,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
@@ -18733,13 +19179,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -18759,306 +19198,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -19194,10 +19337,111 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -19218,6 +19462,208 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -19251,13 +19697,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5592535</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -19306,13 +19752,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2081893</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2081893</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -19361,13 +19807,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>27213</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>285749</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>653142</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>54428</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -19444,13 +19890,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1325336</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2081892</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>68036</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -19527,13 +19973,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1115785</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1959429</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -19610,13 +20056,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1132113</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>179615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1975757</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>247651</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -19693,13 +20139,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1718502</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>235322</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121573</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>122464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -19737,13 +20183,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1700892</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>149677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2231571</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>149934</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -28674,19 +29120,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFEF1B00-87E8-47C7-B380-C546B04D75E0}" name="Table1" displayName="Table1" ref="U29:X40" totalsRowShown="0" headerRowDxfId="25" dataDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFEF1B00-87E8-47C7-B380-C546B04D75E0}" name="Table1" displayName="Table1" ref="U29:X40" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{48413587-F8A1-4E93-8B56-0674A2BA276D}" name="Number" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{F29632EC-6CF2-435A-BFAA-0EE3A7E4D13E}" name="Full Name" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{07FDC0CE-213F-4444-B4DC-A87C9D713170}" name="Department" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{4124B5AE-E29D-4C19-B963-F973B708A891}" name="Shifts" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{48413587-F8A1-4E93-8B56-0674A2BA276D}" name="Number" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{F29632EC-6CF2-435A-BFAA-0EE3A7E4D13E}" name="Full Name" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{07FDC0CE-213F-4444-B4DC-A87C9D713170}" name="Department" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{4124B5AE-E29D-4C19-B963-F973B708A891}" name="Shifts" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3FC33EE2-DF9A-4F82-A4DB-04B170B7F510}" name="Table13" displayName="Table13" ref="U74:V85" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" headerRowBorderDxfId="21" tableBorderDxfId="22" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3FC33EE2-DF9A-4F82-A4DB-04B170B7F510}" name="Table13" displayName="Table13" ref="U74:V85" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{50FE3E12-1851-435D-AF07-FBF5AD5D78A8}" name="Number" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{689857E4-A1DE-477F-A18A-7AE8214F8320}" name="Shifts" dataDxfId="18"/>
@@ -28696,7 +29142,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35E1E40D-4F26-4D7E-83FE-4AD2C12E3F95}" name="Table14" displayName="Table14" ref="U137:X148" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35E1E40D-4F26-4D7E-83FE-4AD2C12E3F95}" name="Table14" displayName="Table14" ref="U137:X148" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4C107CE8-E417-4F66-86CF-86B4BE25297A}" name="Number" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{4801C83C-97E2-4871-B133-AD96AB11DDFF}" name="Department Name" dataDxfId="11"/>
@@ -28708,7 +29154,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A35CE68F-1995-4EC3-928A-B18BCA06FE90}" name="Table145" displayName="Table145" ref="U237:X248" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A35CE68F-1995-4EC3-928A-B18BCA06FE90}" name="Table145" displayName="Table145" ref="U237:X248" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7E415F82-DC84-4BEF-9352-5D67522F3979}" name="Number" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{672D7E62-310D-4CCE-931C-F88CA0B2FF00}" name="User Name" dataDxfId="2"/>
@@ -29039,24 +29485,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="33" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="2">
@@ -29184,45 +29630,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D590761D-F943-4F62-9D7E-2F780046D002}">
-  <dimension ref="B3:C5"/>
+  <dimension ref="B3:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="29"/>
-    <col min="3" max="3" width="72.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="39"/>
+    <col min="3" max="3" width="112.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" style="43" customWidth="1"/>
+    <col min="5" max="5" width="47" style="38" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" s="29">
+    <row r="3" spans="2:6">
+      <c r="B3" s="39">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="29">
+    <row r="5" spans="2:6">
+      <c r="B5" s="39">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>117</v>
       </c>
     </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="39">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="39">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="11" spans="2:6" ht="36" customHeight="1" thickBot="1">
+      <c r="B11" s="39">
+        <v>5</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="48"/>
+    </row>
+    <row r="12" spans="2:6" ht="37.5" customHeight="1">
+      <c r="C12" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="18.75">
+      <c r="C13" s="40"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="18.75">
+      <c r="C14" s="40"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="37.5">
+      <c r="C15" s="40"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="112.5">
+      <c r="C16" s="40"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30.75" thickBot="1">
+      <c r="C17" s="40"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="18.75">
+      <c r="C18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+    </row>
+    <row r="19" spans="2:6" ht="18.75">
+      <c r="C19" s="40"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="C20" s="40"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="C21" s="40"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="C22" s="40"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="C23" s="40"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="C24" s="40"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="C25" s="40"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="C26" s="40"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="C27" s="40"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="C28" s="40"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="C29" s="40"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="C30" s="40"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="39">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:C30"/>
+    <mergeCell ref="D12:D17"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F17" r:id="rId1" xr:uid="{CD181404-63B1-47A0-9615-8BA4CDF49397}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EE3C6F-F1AB-4964-B0F0-4C79988ED97F}">
-  <dimension ref="A2:K48"/>
+  <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -29251,132 +29855,133 @@
     </row>
     <row r="4" spans="2:11" ht="24" thickBot="1"/>
     <row r="5" spans="2:11">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="34" t="s">
         <v>88</v>
       </c>
       <c r="C5" s="20"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="26"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="26"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="35"/>
+      <c r="C8" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="26"/>
-      <c r="C8" s="22" t="s">
+    <row r="9" spans="2:11">
+      <c r="B9" s="35"/>
+      <c r="C9" s="22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="24" thickBot="1">
-      <c r="B9" s="27"/>
-      <c r="C9" s="23"/>
+    <row r="10" spans="2:11" ht="24" thickBot="1">
+      <c r="B10" s="36"/>
+      <c r="C10" s="23"/>
     </row>
-    <row r="14" spans="2:11" ht="24" thickBot="1"/>
-    <row r="15" spans="2:11">
-      <c r="B15" s="25" t="s">
+    <row r="15" spans="2:11" ht="24" thickBot="1"/>
+    <row r="16" spans="2:11">
+      <c r="B16" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="E15" s="25" t="s">
+      <c r="C16" s="20"/>
+      <c r="E16" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="20"/>
+      <c r="F16" s="20"/>
     </row>
-    <row r="16" spans="2:11">
-      <c r="B16" s="26"/>
-      <c r="C16" s="21" t="s">
+    <row r="17" spans="2:6">
+      <c r="B17" s="35"/>
+      <c r="C17" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="21" t="s">
+      <c r="E17" s="35"/>
+      <c r="F17" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="26"/>
-      <c r="C17" s="22" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="35"/>
+      <c r="C18" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="22" t="s">
+      <c r="E18" s="35"/>
+      <c r="F18" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="26"/>
-      <c r="C18" s="22" t="s">
+    <row r="19" spans="2:6">
+      <c r="B19" s="35"/>
+      <c r="C19" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="22" t="s">
+      <c r="E19" s="35"/>
+      <c r="F19" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="24" thickBot="1">
-      <c r="B19" s="27"/>
-      <c r="C19" s="23"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="22" t="s">
+    <row r="20" spans="2:6" ht="24" thickBot="1">
+      <c r="B20" s="36"/>
+      <c r="C20" s="23"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="E20" s="26"/>
-      <c r="F20" s="22" t="s">
+    <row r="21" spans="2:6">
+      <c r="E21" s="35"/>
+      <c r="F21" s="22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="24" thickBot="1">
-      <c r="E21" s="27"/>
-      <c r="F21" s="23"/>
+    <row r="22" spans="2:6" ht="24" thickBot="1">
+      <c r="E22" s="36"/>
+      <c r="F22" s="23"/>
     </row>
-    <row r="25" spans="2:6" ht="24" thickBot="1"/>
-    <row r="26" spans="2:6">
-      <c r="E26" s="25" t="s">
+    <row r="26" spans="2:6" ht="24" thickBot="1"/>
+    <row r="27" spans="2:6">
+      <c r="E27" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F27" s="20"/>
     </row>
-    <row r="27" spans="2:6">
-      <c r="E27" s="26"/>
-      <c r="F27" s="21" t="s">
+    <row r="28" spans="2:6">
+      <c r="E28" s="35"/>
+      <c r="F28" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
-      <c r="E28" s="26"/>
-      <c r="F28" s="22" t="s">
+    <row r="29" spans="2:6">
+      <c r="E29" s="35"/>
+      <c r="F29" s="22" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="15"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="22" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="15"/>
-      <c r="E30" s="26"/>
+      <c r="E30" s="35"/>
       <c r="F30" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="15"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="24" thickBot="1">
-      <c r="B31" s="15"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" ht="24" thickBot="1">
       <c r="B32" s="15"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:4">
       <c r="B33" s="15"/>
@@ -29384,53 +29989,56 @@
     <row r="34" spans="1:4">
       <c r="B34" s="15"/>
     </row>
-    <row r="36" spans="1:4">
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+    <row r="35" spans="1:4">
+      <c r="B35" s="15"/>
     </row>
-    <row r="38" spans="1:4">
-      <c r="C38" s="28"/>
+    <row r="37" spans="1:4">
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="19"/>
-      <c r="C39" s="28"/>
+      <c r="C39" s="37"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="19"/>
+      <c r="C40" s="37"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="C41" s="28"/>
+      <c r="A41" s="19"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="19"/>
-      <c r="C42" s="28"/>
+      <c r="C42" s="37"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="19"/>
+      <c r="C43" s="37"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="C44" s="16"/>
+      <c r="A44" s="19"/>
     </row>
-    <row r="46" spans="1:4">
-      <c r="C46" s="28"/>
+    <row r="45" spans="1:4">
+      <c r="C45" s="16"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="19"/>
-      <c r="C47" s="28"/>
+      <c r="C47" s="37"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="19"/>
-      <c r="D48" s="18"/>
+      <c r="C48" s="37"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="19"/>
+      <c r="D49" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="E15:E21"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E16:E22"/>
+    <mergeCell ref="B16:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -29442,7 +30050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062B95DE-E0B7-4369-91F8-58BF02E69A08}">
   <dimension ref="U29:X248"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R232" sqref="R232"/>
     </sheetView>
   </sheetViews>
@@ -29455,324 +30063,324 @@
   </cols>
   <sheetData>
     <row r="29" spans="21:24">
-      <c r="U29" s="30" t="s">
+      <c r="U29" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="V29" s="31" t="s">
+      <c r="V29" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="W29" s="31" t="s">
+      <c r="W29" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="X29" s="32" t="s">
+      <c r="X29" s="26" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="30" spans="21:24">
-      <c r="U30" s="33" t="s">
+      <c r="U30" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="V30" s="34" t="s">
+      <c r="V30" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="W30" s="34" t="s">
+      <c r="W30" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="X30" s="35" t="s">
+      <c r="X30" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="31" spans="21:24">
-      <c r="U31" s="33"/>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
-      <c r="X31" s="35"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="28"/>
+      <c r="X31" s="29"/>
     </row>
     <row r="32" spans="21:24">
-      <c r="U32" s="33"/>
-      <c r="V32" s="34"/>
-      <c r="W32" s="34"/>
-      <c r="X32" s="35"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="28"/>
+      <c r="W32" s="28"/>
+      <c r="X32" s="29"/>
     </row>
     <row r="33" spans="21:24">
-      <c r="U33" s="33"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
-      <c r="X33" s="35"/>
+      <c r="U33" s="27"/>
+      <c r="V33" s="28"/>
+      <c r="W33" s="28"/>
+      <c r="X33" s="29"/>
     </row>
     <row r="34" spans="21:24">
-      <c r="U34" s="33"/>
-      <c r="V34" s="34"/>
-      <c r="W34" s="34"/>
-      <c r="X34" s="35"/>
+      <c r="U34" s="27"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="29"/>
     </row>
     <row r="35" spans="21:24">
-      <c r="U35" s="33"/>
-      <c r="V35" s="34"/>
-      <c r="W35" s="34"/>
-      <c r="X35" s="35"/>
+      <c r="U35" s="27"/>
+      <c r="V35" s="28"/>
+      <c r="W35" s="28"/>
+      <c r="X35" s="29"/>
     </row>
     <row r="36" spans="21:24">
-      <c r="U36" s="33"/>
-      <c r="V36" s="34"/>
-      <c r="W36" s="34"/>
-      <c r="X36" s="35"/>
+      <c r="U36" s="27"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="28"/>
+      <c r="X36" s="29"/>
     </row>
     <row r="37" spans="21:24">
-      <c r="U37" s="33"/>
-      <c r="V37" s="34"/>
-      <c r="W37" s="34"/>
-      <c r="X37" s="35"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="28"/>
+      <c r="X37" s="29"/>
     </row>
     <row r="38" spans="21:24">
-      <c r="U38" s="33"/>
-      <c r="V38" s="34"/>
-      <c r="W38" s="34"/>
-      <c r="X38" s="35"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="28"/>
+      <c r="X38" s="29"/>
     </row>
     <row r="39" spans="21:24">
-      <c r="U39" s="33"/>
-      <c r="V39" s="34"/>
-      <c r="W39" s="34"/>
-      <c r="X39" s="35"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="29"/>
     </row>
     <row r="40" spans="21:24">
-      <c r="U40" s="36"/>
-      <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="38"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="31"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="32"/>
     </row>
     <row r="74" spans="21:22">
-      <c r="U74" s="30" t="s">
+      <c r="U74" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="V74" s="32" t="s">
+      <c r="V74" s="26" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="75" spans="21:22">
-      <c r="U75" s="33" t="s">
+      <c r="U75" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="V75" s="35" t="s">
+      <c r="V75" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="76" spans="21:22">
-      <c r="U76" s="33"/>
-      <c r="V76" s="35"/>
+      <c r="U76" s="27"/>
+      <c r="V76" s="29"/>
     </row>
     <row r="77" spans="21:22">
-      <c r="U77" s="33"/>
-      <c r="V77" s="35"/>
+      <c r="U77" s="27"/>
+      <c r="V77" s="29"/>
     </row>
     <row r="78" spans="21:22">
-      <c r="U78" s="33"/>
-      <c r="V78" s="35"/>
+      <c r="U78" s="27"/>
+      <c r="V78" s="29"/>
     </row>
     <row r="79" spans="21:22">
-      <c r="U79" s="33"/>
-      <c r="V79" s="35"/>
+      <c r="U79" s="27"/>
+      <c r="V79" s="29"/>
     </row>
     <row r="80" spans="21:22">
-      <c r="U80" s="33"/>
-      <c r="V80" s="35"/>
+      <c r="U80" s="27"/>
+      <c r="V80" s="29"/>
     </row>
     <row r="81" spans="21:22">
-      <c r="U81" s="33"/>
-      <c r="V81" s="35"/>
+      <c r="U81" s="27"/>
+      <c r="V81" s="29"/>
     </row>
     <row r="82" spans="21:22">
-      <c r="U82" s="33"/>
-      <c r="V82" s="35"/>
+      <c r="U82" s="27"/>
+      <c r="V82" s="29"/>
     </row>
     <row r="83" spans="21:22">
-      <c r="U83" s="33"/>
-      <c r="V83" s="35"/>
+      <c r="U83" s="27"/>
+      <c r="V83" s="29"/>
     </row>
     <row r="84" spans="21:22">
-      <c r="U84" s="33"/>
-      <c r="V84" s="35"/>
+      <c r="U84" s="27"/>
+      <c r="V84" s="29"/>
     </row>
     <row r="85" spans="21:22">
-      <c r="U85" s="36"/>
-      <c r="V85" s="38"/>
+      <c r="U85" s="30"/>
+      <c r="V85" s="32"/>
     </row>
     <row r="137" spans="21:24">
-      <c r="U137" s="30" t="s">
+      <c r="U137" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="V137" s="31" t="s">
+      <c r="V137" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="W137" s="31" t="s">
+      <c r="W137" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="X137" s="32" t="s">
+      <c r="X137" s="26" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="138" spans="21:24">
-      <c r="U138" s="33" t="s">
+      <c r="U138" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="V138" s="34" t="s">
+      <c r="V138" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="W138" s="34" t="s">
+      <c r="W138" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="X138" s="35" t="s">
+      <c r="X138" s="29" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="139" spans="21:24">
-      <c r="U139" s="33"/>
-      <c r="V139" s="34"/>
-      <c r="W139" s="34"/>
-      <c r="X139" s="35"/>
+      <c r="U139" s="27"/>
+      <c r="V139" s="28"/>
+      <c r="W139" s="28"/>
+      <c r="X139" s="29"/>
     </row>
     <row r="140" spans="21:24">
-      <c r="U140" s="33"/>
-      <c r="V140" s="34"/>
-      <c r="W140" s="34"/>
-      <c r="X140" s="35"/>
+      <c r="U140" s="27"/>
+      <c r="V140" s="28"/>
+      <c r="W140" s="28"/>
+      <c r="X140" s="29"/>
     </row>
     <row r="141" spans="21:24">
-      <c r="U141" s="33"/>
-      <c r="V141" s="34"/>
-      <c r="W141" s="34"/>
-      <c r="X141" s="35"/>
+      <c r="U141" s="27"/>
+      <c r="V141" s="28"/>
+      <c r="W141" s="28"/>
+      <c r="X141" s="29"/>
     </row>
     <row r="142" spans="21:24">
-      <c r="U142" s="33"/>
-      <c r="V142" s="34"/>
-      <c r="W142" s="34"/>
-      <c r="X142" s="35"/>
+      <c r="U142" s="27"/>
+      <c r="V142" s="28"/>
+      <c r="W142" s="28"/>
+      <c r="X142" s="29"/>
     </row>
     <row r="143" spans="21:24">
-      <c r="U143" s="33"/>
-      <c r="V143" s="34"/>
-      <c r="W143" s="34"/>
-      <c r="X143" s="35"/>
+      <c r="U143" s="27"/>
+      <c r="V143" s="28"/>
+      <c r="W143" s="28"/>
+      <c r="X143" s="29"/>
     </row>
     <row r="144" spans="21:24">
-      <c r="U144" s="33"/>
-      <c r="V144" s="34"/>
-      <c r="W144" s="34"/>
-      <c r="X144" s="35"/>
+      <c r="U144" s="27"/>
+      <c r="V144" s="28"/>
+      <c r="W144" s="28"/>
+      <c r="X144" s="29"/>
     </row>
     <row r="145" spans="21:24">
-      <c r="U145" s="33"/>
-      <c r="V145" s="34"/>
-      <c r="W145" s="34"/>
-      <c r="X145" s="35"/>
+      <c r="U145" s="27"/>
+      <c r="V145" s="28"/>
+      <c r="W145" s="28"/>
+      <c r="X145" s="29"/>
     </row>
     <row r="146" spans="21:24">
-      <c r="U146" s="33"/>
-      <c r="V146" s="34"/>
-      <c r="W146" s="34"/>
-      <c r="X146" s="35"/>
+      <c r="U146" s="27"/>
+      <c r="V146" s="28"/>
+      <c r="W146" s="28"/>
+      <c r="X146" s="29"/>
     </row>
     <row r="147" spans="21:24">
-      <c r="U147" s="33"/>
-      <c r="V147" s="34"/>
-      <c r="W147" s="34"/>
-      <c r="X147" s="35"/>
+      <c r="U147" s="27"/>
+      <c r="V147" s="28"/>
+      <c r="W147" s="28"/>
+      <c r="X147" s="29"/>
     </row>
     <row r="148" spans="21:24">
-      <c r="U148" s="36"/>
-      <c r="V148" s="37"/>
-      <c r="W148" s="37"/>
-      <c r="X148" s="38"/>
+      <c r="U148" s="30"/>
+      <c r="V148" s="31"/>
+      <c r="W148" s="31"/>
+      <c r="X148" s="32"/>
     </row>
     <row r="237" spans="21:24">
-      <c r="U237" s="30" t="s">
+      <c r="U237" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="V237" s="31" t="s">
+      <c r="V237" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="W237" s="31" t="s">
+      <c r="W237" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="X237" s="31" t="s">
+      <c r="X237" s="25" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="238" spans="21:24">
-      <c r="U238" s="33" t="s">
+      <c r="U238" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="V238" s="34" t="s">
+      <c r="V238" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="W238" s="34" t="s">
+      <c r="W238" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="X238" s="34" t="s">
+      <c r="X238" s="28" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="239" spans="21:24">
-      <c r="U239" s="33"/>
-      <c r="V239" s="34"/>
-      <c r="W239" s="34"/>
-      <c r="X239" s="35"/>
+      <c r="U239" s="27"/>
+      <c r="V239" s="28"/>
+      <c r="W239" s="28"/>
+      <c r="X239" s="29"/>
     </row>
     <row r="240" spans="21:24">
-      <c r="U240" s="33"/>
-      <c r="V240" s="34"/>
-      <c r="W240" s="34"/>
-      <c r="X240" s="35"/>
+      <c r="U240" s="27"/>
+      <c r="V240" s="28"/>
+      <c r="W240" s="28"/>
+      <c r="X240" s="29"/>
     </row>
     <row r="241" spans="21:24">
-      <c r="U241" s="33"/>
-      <c r="V241" s="34"/>
-      <c r="W241" s="34"/>
-      <c r="X241" s="35"/>
+      <c r="U241" s="27"/>
+      <c r="V241" s="28"/>
+      <c r="W241" s="28"/>
+      <c r="X241" s="29"/>
     </row>
     <row r="242" spans="21:24">
-      <c r="U242" s="33"/>
-      <c r="V242" s="34"/>
-      <c r="W242" s="34"/>
-      <c r="X242" s="35"/>
+      <c r="U242" s="27"/>
+      <c r="V242" s="28"/>
+      <c r="W242" s="28"/>
+      <c r="X242" s="29"/>
     </row>
     <row r="243" spans="21:24">
-      <c r="U243" s="33"/>
-      <c r="V243" s="34"/>
-      <c r="W243" s="34"/>
-      <c r="X243" s="35"/>
+      <c r="U243" s="27"/>
+      <c r="V243" s="28"/>
+      <c r="W243" s="28"/>
+      <c r="X243" s="29"/>
     </row>
     <row r="244" spans="21:24">
-      <c r="U244" s="33"/>
-      <c r="V244" s="34"/>
-      <c r="W244" s="34"/>
-      <c r="X244" s="35"/>
+      <c r="U244" s="27"/>
+      <c r="V244" s="28"/>
+      <c r="W244" s="28"/>
+      <c r="X244" s="29"/>
     </row>
     <row r="245" spans="21:24">
-      <c r="U245" s="33"/>
-      <c r="V245" s="34"/>
-      <c r="W245" s="34"/>
-      <c r="X245" s="35"/>
+      <c r="U245" s="27"/>
+      <c r="V245" s="28"/>
+      <c r="W245" s="28"/>
+      <c r="X245" s="29"/>
     </row>
     <row r="246" spans="21:24">
-      <c r="U246" s="33"/>
-      <c r="V246" s="34"/>
-      <c r="W246" s="34"/>
-      <c r="X246" s="35"/>
+      <c r="U246" s="27"/>
+      <c r="V246" s="28"/>
+      <c r="W246" s="28"/>
+      <c r="X246" s="29"/>
     </row>
     <row r="247" spans="21:24">
-      <c r="U247" s="33"/>
-      <c r="V247" s="34"/>
-      <c r="W247" s="34"/>
-      <c r="X247" s="35"/>
+      <c r="U247" s="27"/>
+      <c r="V247" s="28"/>
+      <c r="W247" s="28"/>
+      <c r="X247" s="29"/>
     </row>
     <row r="248" spans="21:24">
-      <c r="U248" s="36"/>
-      <c r="V248" s="37"/>
-      <c r="W248" s="37"/>
-      <c r="X248" s="38"/>
+      <c r="U248" s="30"/>
+      <c r="V248" s="31"/>
+      <c r="W248" s="31"/>
+      <c r="X248" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Third commit 4-10-23 - Finish the Employees and Department pages include edit and add method - But without delete - again push
</commit_message>
<xml_diff>
--- a/Data base structure.xlsx
+++ b/Data base structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\NodeJS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A415B-E421-497C-ACBC-14CE1B7D7E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EF1131-5B40-4222-BF9C-5703CCCE7A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="2" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
   <si>
     <t>נושא</t>
   </si>
@@ -17700,6 +17700,9 @@
     <t>employee schema</t>
   </si>
   <si>
+    <t>Shift schema</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -17709,7 +17712,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>DepartmentID</t>
+      <t>Full Name</t>
     </r>
     <r>
       <rPr>
@@ -17719,7 +17722,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : </t>
+      <t xml:space="preserve"> :{ type: </t>
     </r>
     <r>
       <rPr>
@@ -17730,11 +17733,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(reference to department id)</t>
-    </r>
-  </si>
-  <si>
-    <t>Shift schema</t>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, required: true },</t>
+    </r>
   </si>
   <si>
     <r>
@@ -17746,7 +17756,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Full Name</t>
+      <t>Num Of Actions</t>
     </r>
     <r>
       <rPr>
@@ -17767,7 +17777,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>String</t>
+      <t>Number</t>
     </r>
     <r>
       <rPr>
@@ -17790,7 +17800,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Num Of Actions</t>
+      <t>Name</t>
     </r>
     <r>
       <rPr>
@@ -17811,7 +17821,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Number</t>
+      <t>String</t>
     </r>
     <r>
       <rPr>
@@ -17834,7 +17844,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Name</t>
+      <t>Manager</t>
     </r>
     <r>
       <rPr>
@@ -17844,7 +17854,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> :{ type: </t>
+      <t xml:space="preserve"> : </t>
     </r>
     <r>
       <rPr>
@@ -17855,139 +17865,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>String</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, required: true },</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Manager</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>(reference to emloyee id)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Last Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :{ type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>String</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, required: true },</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Start Work Year</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :{ type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, required: true },</t>
     </r>
   </si>
   <si>
@@ -18126,50 +18004,6 @@
     <t>npm i express cors jsonwebtoken mongoose dotenv bcryptjs</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>First Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :{ type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>String</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, required: true },</t>
-    </r>
-  </si>
-  <si>
     <t>npm install express-session cookie-parser</t>
   </si>
   <si>
@@ -18354,6 +18188,206 @@
   </si>
   <si>
     <t>npm i jsonfile</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>startWorkYear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :{ type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, required: true },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>firstName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :{ type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, required: true },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lastName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :{ type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, required: true },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>department</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(reference to department id)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shiftsArr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(reference to Shift id)]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -19011,29 +19045,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -19044,19 +19060,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -19076,6 +19083,33 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -19752,13 +19786,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2081893</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2081893</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -19973,13 +20007,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1115785</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1959429</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -20056,13 +20090,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1132113</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>179615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1975757</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>247651</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -20139,13 +20173,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1718502</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>235322</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121573</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>122464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -20183,13 +20217,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1700892</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>149677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2231571</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>149934</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -21338,15 +21372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>145674</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:colOff>168086</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>43141</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>121584</xdr:rowOff>
+      <xdr:colOff>65553</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>65554</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -21376,7 +21410,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1961027" y="7732059"/>
+          <a:off x="1983439" y="8628529"/>
           <a:ext cx="4133290" cy="2295525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -21399,15 +21433,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>123264</xdr:rowOff>
+      <xdr:colOff>280148</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>67234</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>421341</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:colOff>443753</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -21422,7 +21456,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5098677" y="7171764"/>
+          <a:off x="5121089" y="8068234"/>
           <a:ext cx="768723" cy="324971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -21464,15 +21498,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>504265</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100853</xdr:rowOff>
+      <xdr:colOff>526677</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>437030</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:colOff>459442</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -21487,7 +21521,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3529853" y="7339853"/>
+          <a:off x="3552265" y="8236323"/>
           <a:ext cx="1748118" cy="369794"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -21517,15 +21551,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>291352</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>123265</xdr:rowOff>
+      <xdr:colOff>313764</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>437030</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>100853</xdr:rowOff>
+      <xdr:colOff>459442</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -21540,7 +21574,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4527176" y="7362265"/>
+          <a:off x="4549588" y="8258735"/>
           <a:ext cx="750795" cy="358588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -24189,16 +24223,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>417420</xdr:colOff>
-      <xdr:row>170</xdr:row>
-      <xdr:rowOff>155762</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>372597</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>54909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>45945</xdr:colOff>
-      <xdr:row>182</xdr:row>
-      <xdr:rowOff>165287</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1122</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>64434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -24228,8 +24262,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7123020" y="32540762"/>
-          <a:ext cx="2066925" cy="2295525"/>
+          <a:off x="10054479" y="32630409"/>
+          <a:ext cx="2048996" cy="2295525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -27165,15 +27199,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>150161</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>162543</xdr:rowOff>
+      <xdr:colOff>168087</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95308</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>593912</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>71630</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>4395</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -27201,8 +27235,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1965514" y="10449543"/>
-          <a:ext cx="2259104" cy="480587"/>
+          <a:off x="1983440" y="7715308"/>
+          <a:ext cx="3350560" cy="480587"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -27223,16 +27257,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>103558</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>50256</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>134467</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>173521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>300458</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>184727</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>78442</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>117492</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -27247,8 +27281,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1313793" y="10527756"/>
-          <a:ext cx="3222489" cy="324971"/>
+          <a:off x="1949820" y="7793521"/>
+          <a:ext cx="2969563" cy="324971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -27281,6 +27315,11 @@
             <a:rPr lang="en-US" sz="1100" b="0" u="sng"/>
             <a:t>DropDown to filter employees</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t> by departments</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="sng"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -29485,24 +29524,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="46" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="2">
@@ -29638,174 +29677,174 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="39"/>
+    <col min="2" max="2" width="9.140625" style="34"/>
     <col min="3" max="3" width="112.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14" style="43" customWidth="1"/>
-    <col min="5" max="5" width="47" style="38" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="14" style="37" customWidth="1"/>
+    <col min="5" max="5" width="47" style="33" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="39">
+      <c r="B3" s="34">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="39">
+      <c r="B5" s="34">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="39">
+      <c r="B7" s="34">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="39">
+      <c r="B9" s="34">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="11" spans="2:6" ht="36" customHeight="1" thickBot="1">
-      <c r="B11" s="39">
+      <c r="B11" s="34">
         <v>5</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>122</v>
+      <c r="C11" s="45" t="s">
+        <v>118</v>
       </c>
-      <c r="D11" s="41" t="s">
-        <v>123</v>
+      <c r="D11" s="35" t="s">
+        <v>119</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F11" s="48"/>
     </row>
     <row r="12" spans="2:6" ht="37.5" customHeight="1">
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="F12" s="44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="18.75">
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="52" t="s">
+    </row>
+    <row r="14" spans="2:6" ht="18.75">
+      <c r="C14" s="49"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="37.5">
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F15" s="38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="18.75">
-      <c r="C13" s="40"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="18.75">
-      <c r="C14" s="40"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="51" t="s">
+    <row r="16" spans="2:6" ht="112.5">
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F16" s="38" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="37.5">
-      <c r="C15" s="40"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="51" t="s">
+    <row r="17" spans="2:6" ht="30.75" thickBot="1">
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F17" s="41" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="112.5">
-      <c r="C16" s="40"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="45" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="30.75" thickBot="1">
-      <c r="C17" s="40"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>137</v>
-      </c>
-    </row>
     <row r="18" spans="2:6" ht="18.75">
-      <c r="C18" s="40"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="C18" s="49"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="2:6" ht="18.75">
-      <c r="C19" s="40"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="C19" s="49"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="C20" s="40"/>
+      <c r="C20" s="49"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="C21" s="40"/>
+      <c r="C21" s="49"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="C22" s="40"/>
+      <c r="C22" s="49"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="C23" s="40"/>
+      <c r="C23" s="49"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="C24" s="40"/>
+      <c r="C24" s="49"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="C25" s="40"/>
+      <c r="C25" s="49"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="C26" s="40"/>
+      <c r="C26" s="49"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="C27" s="40"/>
+      <c r="C27" s="49"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="C28" s="40"/>
+      <c r="C28" s="49"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="C29" s="40"/>
+      <c r="C29" s="49"/>
     </row>
     <row r="30" spans="2:6">
-      <c r="C30" s="40"/>
+      <c r="C30" s="49"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="39">
+      <c r="B32" s="34">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -29823,10 +29862,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EE3C6F-F1AB-4964-B0F0-4C79988ED97F}">
-  <dimension ref="A2:K49"/>
+  <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -29855,189 +29894,195 @@
     </row>
     <row r="4" spans="2:11" ht="24" thickBot="1"/>
     <row r="5" spans="2:11">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="51" t="s">
         <v>88</v>
       </c>
       <c r="C5" s="20"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="35"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="35"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="21"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="35"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="52"/>
+      <c r="C9" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="35"/>
-      <c r="C9" s="22" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="10" spans="2:11" ht="24" thickBot="1">
-      <c r="B10" s="36"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="23"/>
     </row>
     <row r="15" spans="2:11" ht="24" thickBot="1"/>
     <row r="16" spans="2:11">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="51" t="s">
         <v>89</v>
       </c>
       <c r="C16" s="20"/>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="51" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="20"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="35"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="35"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="22" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="35"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="22" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="24" thickBot="1">
-      <c r="B20" s="36"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="23"/>
-      <c r="E20" s="35"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="22" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="E21" s="35"/>
+      <c r="E21" s="52"/>
       <c r="F21" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="E22" s="52"/>
+      <c r="F22" s="22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="24" thickBot="1">
+      <c r="E23" s="53"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="27" spans="2:6" ht="24" thickBot="1"/>
+    <row r="28" spans="2:6">
+      <c r="E28" s="51" t="s">
         <v>92</v>
       </c>
+      <c r="F28" s="20"/>
     </row>
-    <row r="22" spans="2:6" ht="24" thickBot="1">
-      <c r="E22" s="36"/>
-      <c r="F22" s="23"/>
-    </row>
-    <row r="26" spans="2:6" ht="24" thickBot="1"/>
-    <row r="27" spans="2:6">
-      <c r="E27" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="20"/>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="E28" s="35"/>
-      <c r="F28" s="21" t="s">
+    <row r="29" spans="2:6">
+      <c r="E29" s="52"/>
+      <c r="F29" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
-      <c r="E29" s="35"/>
-      <c r="F29" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="15"/>
-      <c r="E30" s="35"/>
+      <c r="E30" s="52"/>
       <c r="F30" s="22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="15"/>
-      <c r="E31" s="35"/>
+      <c r="E31" s="52"/>
       <c r="F31" s="22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="24" thickBot="1">
+    <row r="32" spans="2:6">
       <c r="B32" s="15"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="23"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="22" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6" ht="24" thickBot="1">
       <c r="B33" s="15"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="23"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="B34" s="15"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:6">
       <c r="B35" s="15"/>
     </row>
-    <row r="37" spans="1:4">
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
+    <row r="36" spans="1:6">
+      <c r="B36" s="15"/>
     </row>
-    <row r="39" spans="1:4">
-      <c r="C39" s="37"/>
+    <row r="38" spans="1:6">
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="19"/>
-      <c r="C40" s="37"/>
+    <row r="40" spans="1:6">
+      <c r="C40" s="54"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:6">
       <c r="A41" s="19"/>
+      <c r="C41" s="54"/>
     </row>
-    <row r="42" spans="1:4">
-      <c r="C42" s="37"/>
+    <row r="42" spans="1:6">
+      <c r="A42" s="19"/>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="19"/>
-      <c r="C43" s="37"/>
+    <row r="43" spans="1:6">
+      <c r="C43" s="54"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:6">
       <c r="A44" s="19"/>
+      <c r="C44" s="54"/>
     </row>
-    <row r="45" spans="1:4">
-      <c r="C45" s="16"/>
+    <row r="45" spans="1:6">
+      <c r="A45" s="19"/>
     </row>
-    <row r="47" spans="1:4">
-      <c r="C47" s="37"/>
+    <row r="46" spans="1:6">
+      <c r="C46" s="16"/>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="19"/>
-      <c r="C48" s="37"/>
+    <row r="48" spans="1:6">
+      <c r="C48" s="54"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="19"/>
-      <c r="D49" s="18"/>
+      <c r="C49" s="54"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="19"/>
+      <c r="D50" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B5:B10"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E16:E22"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="E28:E33"/>
+    <mergeCell ref="E16:E23"/>
     <mergeCell ref="B16:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30050,8 +30095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062B95DE-E0B7-4369-91F8-58BF02E69A08}">
   <dimension ref="U29:X248"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R232" sqref="R232"/>
+    <sheetView topLeftCell="A157" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U175" sqref="U175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30064,30 +30109,30 @@
   <sheetData>
     <row r="29" spans="21:24">
       <c r="U29" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="W29" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="X29" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="21:24">
       <c r="U30" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V30" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="W30" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="X30" s="29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="21:24">
@@ -30152,18 +30197,18 @@
     </row>
     <row r="74" spans="21:22">
       <c r="U74" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V74" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="21:22">
       <c r="U75" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V75" s="29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="21:22">
@@ -30208,30 +30253,30 @@
     </row>
     <row r="137" spans="21:24">
       <c r="U137" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V137" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="W137" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X137" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="138" spans="21:24">
       <c r="U138" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V138" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="W138" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="X138" s="29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="139" spans="21:24">
@@ -30296,30 +30341,30 @@
     </row>
     <row r="237" spans="21:24">
       <c r="U237" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V237" s="25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="W237" s="25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="X237" s="25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="238" spans="21:24">
       <c r="U238" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V238" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="W238" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="X238" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="239" spans="21:24">

</xml_diff>

<commit_message>
Complete the shifts page
</commit_message>
<xml_diff>
--- a/Data base structure.xlsx
+++ b/Data base structure.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\NodeJS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EF1131-5B40-4222-BF9C-5703CCCE7A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B668513-0E36-40EE-BE8F-90D5C4108446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="2" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="1" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
   <sheets>
-    <sheet name="משימות" sheetId="4" r:id="rId1"/>
-    <sheet name="initial Website" sheetId="7" r:id="rId2"/>
-    <sheet name="data base structure" sheetId="5" r:id="rId3"/>
-    <sheet name="Pages" sheetId="6" r:id="rId4"/>
+    <sheet name="initial Website" sheetId="7" r:id="rId1"/>
+    <sheet name="data base structure" sheetId="5" r:id="rId2"/>
+    <sheet name="Pages" sheetId="6" r:id="rId3"/>
+    <sheet name="lookup example" sheetId="8" r:id="rId4"/>
     <sheet name="initial data" sheetId="3" r:id="rId5"/>
+    <sheet name="משימות" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">משימות!$A$3:$E$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">משימות!$A$3:$E$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="157">
   <si>
     <t>נושא</t>
   </si>
@@ -18389,12 +18390,143 @@
       <t>(reference to Shift id)]</t>
     </r>
   </si>
+  <si>
+    <t>Mongodb aggregate $lookup $project and $match do not work [duplicate]</t>
+  </si>
+  <si>
+    <t>I need your help. I am practicing very simple join method with filter on my two collection. It works without filter. My mongodb query is mention below.
+Two Collection</t>
+  </si>
+  <si>
+    <t>First collection</t>
+  </si>
+  <si>
+    <t>{
+    "_id": ObjectId("5ea18cd00715f152a6fcee24"),
+    "company_name": "COMPANY 1",
+    "company_detail_id": [
+            {
+                "_id": ObjectId("5e5db61dbb9d1523f7d78e65") //NOTE: company_detail_id == programs._id
+            }
+    ],
+    "is_deleted": false,
+}</t>
+  </si>
+  <si>
+    <t>Second Collection</t>
+  </si>
+  <si>
+    <t>{
+     "_id": ObjectId("5e5db61dbb9d1523f7d78e65"),
+     "name": "PROGRAM 1",
+     "is_deleted": false
+}</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>var list = await dataModel.aggregate([
+            {
+                $lookup: {
+                    from: "company_details",
+                    localField: "company_detail_id._id",
+                    foreignField: "_id",
+                    as: "programs"
+                }
+            },
+            {
+                "$project": {
+                            "_id": true,
+                            "company_name": true,
+                            "company_detail_id": true,
+                            "is_deleted": true,
+                            "programs._id": true,
+                            "programs.name": true,
+                            "programs.is_deleted": true
+                        }
+            },
+            {
+                "$match": {
+                            "_id": "5ea18cd00715f152a6fcee24",
+                            "is_deleted":false
+                            }
+            }
+        ]).skip(0).limit(10);</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>This query WORKS when</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "$match" : {} 
+    or
+    "$match" : { "company_name": "xyz" } </t>
+  </si>
+  <si>
+    <r>
+      <t>This query </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>NOT WORKING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF232629"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> when</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> "$match" : { "_id" : "5ea18cd00715f152a6fcee24" } 
+    or
+    "$match" : { "_id": "5ea18cd00715f152a6fcee24", "is_deleted":false } </t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>{
+    "_id": "5ea18cd00715f152a6fcee24",
+    "company_name": "COMPANY 1",
+    "company_detail_id": [
+            {
+                "_id": "5e5db61dbb9d1523f7d78e65" //NOTE: company_detail_id == programs._id
+            }
+    ],
+    "is_deleted": false,
+    "programs": [
+            {
+                 "_id": "5e5db61dbb9d1523f7d78e65",
+                 "name": "PROGRAM 1",
+                 "is_deleted": false
+            }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>company_details</t>
+  </si>
+  <si>
+    <t>dataModel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18581,6 +18713,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF232629"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF232629"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF232629"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="10">
@@ -18947,7 +19104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -19110,6 +19267,25 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -29500,179 +29676,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF8076A-65A2-4B83-895F-0776A626122A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D590761D-F943-4F62-9D7E-2F780046D002}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B2:E17"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="83.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1"/>
-    <col min="8" max="8" width="23.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="15" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5">
-      <c r="B2" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="2">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="2">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="2">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="2">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="2">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="2">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="2">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="2">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="2">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="2">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D590761D-F943-4F62-9D7E-2F780046D002}">
   <dimension ref="B3:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29860,12 +29871,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EE3C6F-F1AB-4964-B0F0-4C79988ED97F}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -30091,12 +30105,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062B95DE-E0B7-4369-91F8-58BF02E69A08}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
   <dimension ref="U29:X248"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U175" sqref="U175"/>
+    <sheetView topLeftCell="A190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R212" sqref="R212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30439,10 +30456,119 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EE4ACC-C4E2-48D6-BF1A-E49FAFCB557A}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="B3:B36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="162" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" s="55" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="45">
+      <c r="B6" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="16.5">
+      <c r="B9" s="56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="61" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="150">
+      <c r="B11" s="57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="16.5">
+      <c r="B14" s="56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="75">
+      <c r="B16" s="57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="16.5">
+      <c r="B19" s="56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="405">
+      <c r="B21" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="16.5">
+      <c r="B23" s="56" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="16.5">
+      <c r="B25" s="58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="45">
+      <c r="B27" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="16.5">
+      <c r="B29" s="59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="45">
+      <c r="B31" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="60" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="255">
+      <c r="B36" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://stackoverflow.com/questions/61400857/mongodb-aggregate-lookup-project-and-match-do-not-work" xr:uid="{C6EAAB14-D8BA-44C3-B317-E933EFF422E8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D5BDCB-8977-430D-B7D4-9BFC40BC468A}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
   <dimension ref="C3:C105"/>
   <sheetViews>
@@ -30949,4 +31075,172 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF8076A-65A2-4B83-895F-0776A626122A}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.14999847407452621"/>
+  </sheetPr>
+  <dimension ref="B2:E17"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="83.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1"/>
+    <col min="8" max="8" width="23.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="15" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="2">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="2">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="2">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="2">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete the Node JS project - finish users actions and reset views every midnight
</commit_message>
<xml_diff>
--- a/Data base structure.xlsx
+++ b/Data base structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\NodeJS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B668513-0E36-40EE-BE8F-90D5C4108446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D6DD7C-291A-45D0-A69B-C8E5CB5EBAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="1" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="6" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
   <sheets>
     <sheet name="initial Website" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="lookup example" sheetId="8" r:id="rId4"/>
     <sheet name="initial data" sheetId="3" r:id="rId5"/>
     <sheet name="משימות" sheetId="4" r:id="rId6"/>
+    <sheet name="שגיאה באיפוס Session" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">משימות!$A$3:$E$17</definedName>
@@ -19104,7 +19105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -19241,8 +19242,21 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -19268,24 +19282,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -29334,6 +29332,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>143470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C801E51-5138-B264-DC88-2C70221C50E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="533400" y="333970"/>
+          <a:ext cx="9505950" cy="6238280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFEF1B00-87E8-47C7-B380-C546B04D75E0}" name="Table1" displayName="Table1" ref="U29:X40" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <tableColumns count="4">
@@ -29738,16 +29802,16 @@
       <c r="D11" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="F11" s="48"/>
+      <c r="F11" s="53"/>
     </row>
     <row r="12" spans="2:6" ht="37.5" customHeight="1">
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="55" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="43" t="s">
@@ -29758,8 +29822,8 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.75">
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="42" t="s">
         <v>123</v>
       </c>
@@ -29768,8 +29832,8 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75">
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="42" t="s">
         <v>126</v>
       </c>
@@ -29778,8 +29842,8 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="37.5">
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="42" t="s">
         <v>128</v>
       </c>
@@ -29788,8 +29852,8 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="112.5">
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="42" t="s">
         <v>130</v>
       </c>
@@ -29798,8 +29862,8 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="30.75" thickBot="1">
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="40" t="s">
         <v>132</v>
       </c>
@@ -29808,47 +29872,47 @@
       </c>
     </row>
     <row r="18" spans="2:6" ht="18.75">
-      <c r="C18" s="49"/>
+      <c r="C18" s="54"/>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
     </row>
     <row r="19" spans="2:6" ht="18.75">
-      <c r="C19" s="49"/>
+      <c r="C19" s="54"/>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="C20" s="49"/>
+      <c r="C20" s="54"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="C21" s="49"/>
+      <c r="C21" s="54"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="C22" s="49"/>
+      <c r="C22" s="54"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="C23" s="49"/>
+      <c r="C23" s="54"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="C24" s="49"/>
+      <c r="C24" s="54"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="C25" s="49"/>
+      <c r="C25" s="54"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="C26" s="49"/>
+      <c r="C26" s="54"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="C27" s="49"/>
+      <c r="C27" s="54"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="C28" s="49"/>
+      <c r="C28" s="54"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="C29" s="49"/>
+      <c r="C29" s="54"/>
     </row>
     <row r="30" spans="2:6">
-      <c r="C30" s="49"/>
+      <c r="C30" s="54"/>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="34">
@@ -29878,7 +29942,7 @@
   </sheetPr>
   <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
@@ -29908,138 +29972,138 @@
     </row>
     <row r="4" spans="2:11" ht="24" thickBot="1"/>
     <row r="5" spans="2:11">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="56" t="s">
         <v>88</v>
       </c>
       <c r="C5" s="20"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="52"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="52"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="21"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="52"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="52"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="24" thickBot="1">
-      <c r="B10" s="53"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="23"/>
     </row>
     <row r="15" spans="2:11" ht="24" thickBot="1"/>
     <row r="16" spans="2:11">
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="56" t="s">
         <v>89</v>
       </c>
       <c r="C16" s="20"/>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="56" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="20"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="52"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="52"/>
+      <c r="E17" s="57"/>
       <c r="F17" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="52"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="52"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="22" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="52"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="52"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="22" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="24" thickBot="1">
-      <c r="B20" s="53"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="23"/>
-      <c r="E20" s="52"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="22" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="E21" s="52"/>
+      <c r="E21" s="57"/>
       <c r="F21" s="22" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="E22" s="52"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="22" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="24" thickBot="1">
-      <c r="E23" s="53"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="23"/>
     </row>
     <row r="27" spans="2:6" ht="24" thickBot="1"/>
     <row r="28" spans="2:6">
-      <c r="E28" s="51" t="s">
+      <c r="E28" s="56" t="s">
         <v>92</v>
       </c>
       <c r="F28" s="20"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="E29" s="52"/>
+      <c r="E29" s="57"/>
       <c r="F29" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:6">
-      <c r="E30" s="52"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="15"/>
-      <c r="E31" s="52"/>
+      <c r="E31" s="57"/>
       <c r="F31" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="15"/>
-      <c r="E32" s="52"/>
+      <c r="E32" s="57"/>
       <c r="F32" s="22" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="24" thickBot="1">
       <c r="B33" s="15"/>
-      <c r="E33" s="53"/>
+      <c r="E33" s="58"/>
       <c r="F33" s="23"/>
     </row>
     <row r="34" spans="1:6">
@@ -30056,21 +30120,21 @@
       <c r="D38" s="17"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="C40" s="54"/>
+      <c r="C40" s="59"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="19"/>
-      <c r="C41" s="54"/>
+      <c r="C41" s="59"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="19"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="C43" s="54"/>
+      <c r="C43" s="59"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="19"/>
-      <c r="C44" s="54"/>
+      <c r="C44" s="59"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="19"/>
@@ -30079,11 +30143,11 @@
       <c r="C46" s="16"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="C48" s="54"/>
+      <c r="C48" s="59"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="19"/>
-      <c r="C49" s="54"/>
+      <c r="C49" s="59"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="19"/>
@@ -30473,7 +30537,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:2">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="46" t="s">
         <v>140</v>
       </c>
     </row>
@@ -30483,37 +30547,37 @@
       </c>
     </row>
     <row r="9" spans="2:2" ht="16.5">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="47" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="51" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="150">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="33" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="16.5">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="47" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="51" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="75">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="33" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="16.5">
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="47" t="s">
         <v>146</v>
       </c>
     </row>
@@ -30523,12 +30587,12 @@
       </c>
     </row>
     <row r="23" spans="2:2" ht="16.5">
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="47" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="16.5">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="48" t="s">
         <v>149</v>
       </c>
     </row>
@@ -30538,7 +30602,7 @@
       </c>
     </row>
     <row r="29" spans="2:2" ht="16.5">
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="49" t="s">
         <v>151</v>
       </c>
     </row>
@@ -30548,7 +30612,7 @@
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="50" t="s">
         <v>153</v>
       </c>
     </row>
@@ -31102,24 +31166,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="60" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="2">
@@ -31243,4 +31307,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143C98FA-68DF-475A-8166-946411EBDA91}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete and fix issues in frontend pages, Improving flexibility and efficiency in used the server and use mongodb to stored the session
</commit_message>
<xml_diff>
--- a/Data base structure.xlsx
+++ b/Data base structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\NodeJS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D6DD7C-291A-45D0-A69B-C8E5CB5EBAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9FA4DD-40D8-4191-B358-A5DA55A1B9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="6" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" activeTab="1" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
   <sheets>
     <sheet name="initial Website" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="193">
   <si>
     <t>נושא</t>
   </si>
@@ -18522,12 +18522,789 @@
   <si>
     <t>dataModel</t>
   </si>
+  <si>
+    <t>6512d8dbe5684c73d11f61b2</t>
+  </si>
+  <si>
+    <t>Basheer</t>
+  </si>
+  <si>
+    <t>6512efcec84aa6d8989171bb</t>
+  </si>
+  <si>
+    <t>Maram</t>
+  </si>
+  <si>
+    <t>6512f09fc84aa6d8989171c5</t>
+  </si>
+  <si>
+    <t>Leron</t>
+  </si>
+  <si>
+    <t>6512f0bec84aa6d8989171cf</t>
+  </si>
+  <si>
+    <t>Dorin</t>
+  </si>
+  <si>
+    <t>651a8fef9ec622dd16a6d032</t>
+  </si>
+  <si>
+    <t>Dana</t>
+  </si>
+  <si>
+    <t>652cdc7d0bf134c76c549f41</t>
+  </si>
+  <si>
+    <t>Aviv</t>
+  </si>
+  <si>
+    <t>22. Join two collections using aggregate method lookup to get details - MongoDB</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=naX9Ci0OSCk</t>
+  </si>
+  <si>
+    <t>18/10/23</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: true }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :{ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: true },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>city</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: true }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :{ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: true },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>authorId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="22"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ObjectId:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reference to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> author </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Leele</t>
+  </si>
+  <si>
+    <t>Numbai</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>name:</t>
+  </si>
+  <si>
+    <t>city:</t>
+  </si>
+  <si>
+    <t>authorId:</t>
+  </si>
+  <si>
+    <t>Book 1</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <r>
+      <t>refer to [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Leela</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>db.books.aggregate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>({</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lookup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'authors', </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>localField</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'authorId', </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>foreignField</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"_id", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "authors"}})</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.pretty()</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18740,6 +19517,68 @@
       <color rgb="FFFF0000"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -18797,7 +19636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -19100,12 +19939,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -19154,12 +20017,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -19279,11 +20136,38 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -20346,15 +21230,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1718502</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>235322</xdr:rowOff>
+      <xdr:colOff>208109</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>208108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1121573</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>122464</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5230930</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -20377,7 +21261,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2453288" y="10413465"/>
+          <a:off x="942895" y="7093322"/>
           <a:ext cx="8057214" cy="2281999"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20390,15 +21274,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1700892</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>149677</xdr:rowOff>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2231571</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>149934</xdr:rowOff>
+      <xdr:colOff>721178</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>122720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -20413,7 +21297,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2435678" y="9729106"/>
+          <a:off x="925285" y="6408963"/>
           <a:ext cx="9184822" cy="598971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20447,6 +21331,144 @@
             <a:rPr lang="en-US" sz="2400" b="0" u="sng"/>
             <a:t>Each "Actions" user takes is logged in a json file at the server</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1927411</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>293285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1938617</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>2318</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4873B69D-09C0-42F3-95BF-8B9D9D8FD70E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5691428" y="14534802"/>
+          <a:ext cx="11206" cy="608982"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1053353</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>132870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1896997</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>200906</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D531411-6AB4-43B3-B783-F71A561ADC40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4807324" y="14510017"/>
+          <a:ext cx="843644" cy="359389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="he-IL" sz="1600">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>*.....1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -29752,15 +30774,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="34"/>
+    <col min="2" max="2" width="9.140625" style="32"/>
     <col min="3" max="3" width="112.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14" style="37" customWidth="1"/>
-    <col min="5" max="5" width="47" style="33" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="14" style="35" customWidth="1"/>
+    <col min="5" max="5" width="47" style="31" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="34">
+      <c r="B3" s="32">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -29768,7 +30790,7 @@
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="34">
+      <c r="B5" s="32">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -29776,7 +30798,7 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="34">
+      <c r="B7" s="32">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -29784,7 +30806,7 @@
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="34">
+      <c r="B9" s="32">
         <v>4</v>
       </c>
       <c r="C9" t="s">
@@ -29793,129 +30815,129 @@
     </row>
     <row r="10" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="11" spans="2:6" ht="36" customHeight="1" thickBot="1">
-      <c r="B11" s="34">
+      <c r="B11" s="32">
         <v>5</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="F11" s="53"/>
+      <c r="F11" s="51"/>
     </row>
     <row r="12" spans="2:6" ht="37.5" customHeight="1">
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="42" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.75">
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="42" t="s">
+      <c r="C13" s="52"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="37" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75">
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="42" t="s">
+      <c r="C14" s="52"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="36" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="37.5">
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="42" t="s">
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="36" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="112.5">
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="42" t="s">
+      <c r="C16" s="52"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="36" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="30.75" thickBot="1">
-      <c r="C17" s="54"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="40" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="39" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="18.75">
-      <c r="C18" s="54"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
+      <c r="C18" s="52"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="2:6" ht="18.75">
-      <c r="C19" s="54"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="C19" s="52"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="C20" s="54"/>
+      <c r="C20" s="52"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="C21" s="54"/>
+      <c r="C21" s="52"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="C22" s="54"/>
+      <c r="C22" s="52"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="C23" s="54"/>
+      <c r="C23" s="52"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="C24" s="54"/>
+      <c r="C24" s="52"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="C25" s="54"/>
+      <c r="C25" s="52"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="C26" s="54"/>
+      <c r="C26" s="52"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="C27" s="54"/>
+      <c r="C27" s="52"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="C28" s="54"/>
+      <c r="C28" s="52"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="C29" s="54"/>
+      <c r="C29" s="52"/>
     </row>
     <row r="30" spans="2:6">
-      <c r="C30" s="54"/>
+      <c r="C30" s="52"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="34">
+      <c r="B32" s="32">
         <v>6</v>
       </c>
       <c r="C32" t="s">
@@ -29940,10 +30962,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:K50"/>
+  <dimension ref="A2:K66"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -29972,139 +30994,175 @@
     </row>
     <row r="4" spans="2:11" ht="24" thickBot="1"/>
     <row r="5" spans="2:11">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="18"/>
+      <c r="E5" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="57"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="19" t="s">
         <v>90</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="57"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="19"/>
+      <c r="E7" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="57"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="55"/>
+      <c r="C8" s="20" t="s">
         <v>93</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="57"/>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="20" t="s">
         <v>94</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="24" thickBot="1">
-      <c r="B10" s="58"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="21"/>
+      <c r="E10" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="15" spans="2:11" ht="24" thickBot="1"/>
     <row r="16" spans="2:11">
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="E16" s="56" t="s">
+      <c r="C16" s="18"/>
+      <c r="E16" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="20"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="57"/>
-      <c r="C17" s="21" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="21" t="s">
+      <c r="E17" s="55"/>
+      <c r="F17" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="57"/>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="22" t="s">
+      <c r="E18" s="55"/>
+      <c r="F18" s="20" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="57"/>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="22" t="s">
+      <c r="E19" s="55"/>
+      <c r="F19" s="20" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="24" thickBot="1">
-      <c r="B20" s="58"/>
-      <c r="C20" s="23"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="22" t="s">
+      <c r="B20" s="56"/>
+      <c r="C20" s="21"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="20" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="E21" s="57"/>
-      <c r="F21" s="22" t="s">
+      <c r="E21" s="55"/>
+      <c r="F21" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="E22" s="57"/>
-      <c r="F22" s="22" t="s">
+      <c r="E22" s="55"/>
+      <c r="F22" s="20" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="24" thickBot="1">
-      <c r="E23" s="58"/>
-      <c r="F23" s="23"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="21"/>
     </row>
     <row r="27" spans="2:6" ht="24" thickBot="1"/>
     <row r="28" spans="2:6">
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="20"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="E29" s="57"/>
-      <c r="F29" s="21" t="s">
+      <c r="E29" s="55"/>
+      <c r="F29" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:6">
-      <c r="E30" s="57"/>
-      <c r="F30" s="22" t="s">
+      <c r="E30" s="55"/>
+      <c r="F30" s="20" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="15"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="22" t="s">
+      <c r="E31" s="55"/>
+      <c r="F31" s="20" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="15"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="22" t="s">
+      <c r="E32" s="55"/>
+      <c r="F32" s="20" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="24" thickBot="1">
       <c r="B33" s="15"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="23"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" s="15"/>
@@ -30113,59 +31171,222 @@
       <c r="B35" s="15"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="B36" s="15"/>
+      <c r="B36" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="C38" s="16"/>
-      <c r="D38" s="17"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="E39" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="F39" s="59"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="C40" s="59"/>
+      <c r="E40" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="61"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="19"/>
-      <c r="C41" s="59"/>
+      <c r="A41" s="17"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="19"/>
+      <c r="A42" s="17"/>
     </row>
-    <row r="43" spans="1:6">
-      <c r="C43" s="59"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="19"/>
-      <c r="C44" s="59"/>
+    <row r="44" spans="1:6" ht="24" thickBot="1">
+      <c r="A44" s="17"/>
+      <c r="D44" s="12"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="19"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="C46" s="16"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" s="55"/>
+      <c r="C47" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" s="63"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="C48" s="59"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" s="63"/>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="19"/>
-      <c r="C49" s="59"/>
+    <row r="49" spans="1:6" ht="24" thickBot="1">
+      <c r="A49" s="17"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="63"/>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="19"/>
-      <c r="D50" s="18"/>
+    <row r="50" spans="1:6">
+      <c r="A50" s="17"/>
+      <c r="D50" s="64"/>
+    </row>
+    <row r="51" spans="1:6" ht="24" thickBot="1">
+      <c r="C51" s="16"/>
+      <c r="D51" s="63"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="B52" s="54" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="63"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" s="55"/>
+      <c r="C53" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="63"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="B54" s="55"/>
+      <c r="C54" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="B55" s="55"/>
+      <c r="C55" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" s="15">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="28.5">
+      <c r="B56" s="55"/>
+      <c r="C56" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="24" thickBot="1">
+      <c r="B57" s="56"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="63"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="D58" s="63"/>
+      <c r="E58" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="D59" s="63"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="D60" s="63"/>
+    </row>
+    <row r="61" spans="1:6" ht="24" thickBot="1">
+      <c r="D61" s="63"/>
+    </row>
+    <row r="62" spans="1:6" ht="24" thickBot="1">
+      <c r="B62" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="C62" s="67" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="58"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="B63" s="15"/>
+      <c r="D63" s="63"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="B64" s="15"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="15"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="C62:F62"/>
     <mergeCell ref="B5:B10"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C48:C49"/>
     <mergeCell ref="E28:E33"/>
     <mergeCell ref="E16:E23"/>
     <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="B36:F38"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="B52:B57"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E40" r:id="rId1" xr:uid="{FCF1184A-2F64-498C-99E0-EDC915006B5A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -30189,324 +31410,324 @@
   </cols>
   <sheetData>
     <row r="29" spans="21:24">
-      <c r="U29" s="24" t="s">
+      <c r="U29" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="V29" s="25" t="s">
+      <c r="V29" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="W29" s="25" t="s">
+      <c r="W29" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="X29" s="26" t="s">
+      <c r="X29" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="30" spans="21:24">
-      <c r="U30" s="27" t="s">
+      <c r="U30" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="V30" s="28" t="s">
+      <c r="V30" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="W30" s="28" t="s">
+      <c r="W30" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="X30" s="29" t="s">
+      <c r="X30" s="27" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="31" spans="21:24">
-      <c r="U31" s="27"/>
-      <c r="V31" s="28"/>
-      <c r="W31" s="28"/>
-      <c r="X31" s="29"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="27"/>
     </row>
     <row r="32" spans="21:24">
-      <c r="U32" s="27"/>
-      <c r="V32" s="28"/>
-      <c r="W32" s="28"/>
-      <c r="X32" s="29"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="27"/>
     </row>
     <row r="33" spans="21:24">
-      <c r="U33" s="27"/>
-      <c r="V33" s="28"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="29"/>
+      <c r="U33" s="25"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="27"/>
     </row>
     <row r="34" spans="21:24">
-      <c r="U34" s="27"/>
-      <c r="V34" s="28"/>
-      <c r="W34" s="28"/>
-      <c r="X34" s="29"/>
+      <c r="U34" s="25"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="27"/>
     </row>
     <row r="35" spans="21:24">
-      <c r="U35" s="27"/>
-      <c r="V35" s="28"/>
-      <c r="W35" s="28"/>
-      <c r="X35" s="29"/>
+      <c r="U35" s="25"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="27"/>
     </row>
     <row r="36" spans="21:24">
-      <c r="U36" s="27"/>
-      <c r="V36" s="28"/>
-      <c r="W36" s="28"/>
-      <c r="X36" s="29"/>
+      <c r="U36" s="25"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="27"/>
     </row>
     <row r="37" spans="21:24">
-      <c r="U37" s="27"/>
-      <c r="V37" s="28"/>
-      <c r="W37" s="28"/>
-      <c r="X37" s="29"/>
+      <c r="U37" s="25"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="27"/>
     </row>
     <row r="38" spans="21:24">
-      <c r="U38" s="27"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="29"/>
+      <c r="U38" s="25"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="27"/>
     </row>
     <row r="39" spans="21:24">
-      <c r="U39" s="27"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="29"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="27"/>
     </row>
     <row r="40" spans="21:24">
-      <c r="U40" s="30"/>
-      <c r="V40" s="31"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="32"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="30"/>
     </row>
     <row r="74" spans="21:22">
-      <c r="U74" s="24" t="s">
+      <c r="U74" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="V74" s="26" t="s">
+      <c r="V74" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="75" spans="21:22">
-      <c r="U75" s="27" t="s">
+      <c r="U75" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="V75" s="29" t="s">
+      <c r="V75" s="27" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="76" spans="21:22">
-      <c r="U76" s="27"/>
-      <c r="V76" s="29"/>
+      <c r="U76" s="25"/>
+      <c r="V76" s="27"/>
     </row>
     <row r="77" spans="21:22">
-      <c r="U77" s="27"/>
-      <c r="V77" s="29"/>
+      <c r="U77" s="25"/>
+      <c r="V77" s="27"/>
     </row>
     <row r="78" spans="21:22">
-      <c r="U78" s="27"/>
-      <c r="V78" s="29"/>
+      <c r="U78" s="25"/>
+      <c r="V78" s="27"/>
     </row>
     <row r="79" spans="21:22">
-      <c r="U79" s="27"/>
-      <c r="V79" s="29"/>
+      <c r="U79" s="25"/>
+      <c r="V79" s="27"/>
     </row>
     <row r="80" spans="21:22">
-      <c r="U80" s="27"/>
-      <c r="V80" s="29"/>
+      <c r="U80" s="25"/>
+      <c r="V80" s="27"/>
     </row>
     <row r="81" spans="21:22">
-      <c r="U81" s="27"/>
-      <c r="V81" s="29"/>
+      <c r="U81" s="25"/>
+      <c r="V81" s="27"/>
     </row>
     <row r="82" spans="21:22">
-      <c r="U82" s="27"/>
-      <c r="V82" s="29"/>
+      <c r="U82" s="25"/>
+      <c r="V82" s="27"/>
     </row>
     <row r="83" spans="21:22">
-      <c r="U83" s="27"/>
-      <c r="V83" s="29"/>
+      <c r="U83" s="25"/>
+      <c r="V83" s="27"/>
     </row>
     <row r="84" spans="21:22">
-      <c r="U84" s="27"/>
-      <c r="V84" s="29"/>
+      <c r="U84" s="25"/>
+      <c r="V84" s="27"/>
     </row>
     <row r="85" spans="21:22">
-      <c r="U85" s="30"/>
-      <c r="V85" s="32"/>
+      <c r="U85" s="28"/>
+      <c r="V85" s="30"/>
     </row>
     <row r="137" spans="21:24">
-      <c r="U137" s="24" t="s">
+      <c r="U137" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="V137" s="25" t="s">
+      <c r="V137" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="W137" s="25" t="s">
+      <c r="W137" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="X137" s="26" t="s">
+      <c r="X137" s="24" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="138" spans="21:24">
-      <c r="U138" s="27" t="s">
+      <c r="U138" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="V138" s="28" t="s">
+      <c r="V138" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="W138" s="28" t="s">
+      <c r="W138" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="X138" s="29" t="s">
+      <c r="X138" s="27" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="139" spans="21:24">
-      <c r="U139" s="27"/>
-      <c r="V139" s="28"/>
-      <c r="W139" s="28"/>
-      <c r="X139" s="29"/>
+      <c r="U139" s="25"/>
+      <c r="V139" s="26"/>
+      <c r="W139" s="26"/>
+      <c r="X139" s="27"/>
     </row>
     <row r="140" spans="21:24">
-      <c r="U140" s="27"/>
-      <c r="V140" s="28"/>
-      <c r="W140" s="28"/>
-      <c r="X140" s="29"/>
+      <c r="U140" s="25"/>
+      <c r="V140" s="26"/>
+      <c r="W140" s="26"/>
+      <c r="X140" s="27"/>
     </row>
     <row r="141" spans="21:24">
-      <c r="U141" s="27"/>
-      <c r="V141" s="28"/>
-      <c r="W141" s="28"/>
-      <c r="X141" s="29"/>
+      <c r="U141" s="25"/>
+      <c r="V141" s="26"/>
+      <c r="W141" s="26"/>
+      <c r="X141" s="27"/>
     </row>
     <row r="142" spans="21:24">
-      <c r="U142" s="27"/>
-      <c r="V142" s="28"/>
-      <c r="W142" s="28"/>
-      <c r="X142" s="29"/>
+      <c r="U142" s="25"/>
+      <c r="V142" s="26"/>
+      <c r="W142" s="26"/>
+      <c r="X142" s="27"/>
     </row>
     <row r="143" spans="21:24">
-      <c r="U143" s="27"/>
-      <c r="V143" s="28"/>
-      <c r="W143" s="28"/>
-      <c r="X143" s="29"/>
+      <c r="U143" s="25"/>
+      <c r="V143" s="26"/>
+      <c r="W143" s="26"/>
+      <c r="X143" s="27"/>
     </row>
     <row r="144" spans="21:24">
-      <c r="U144" s="27"/>
-      <c r="V144" s="28"/>
-      <c r="W144" s="28"/>
-      <c r="X144" s="29"/>
+      <c r="U144" s="25"/>
+      <c r="V144" s="26"/>
+      <c r="W144" s="26"/>
+      <c r="X144" s="27"/>
     </row>
     <row r="145" spans="21:24">
-      <c r="U145" s="27"/>
-      <c r="V145" s="28"/>
-      <c r="W145" s="28"/>
-      <c r="X145" s="29"/>
+      <c r="U145" s="25"/>
+      <c r="V145" s="26"/>
+      <c r="W145" s="26"/>
+      <c r="X145" s="27"/>
     </row>
     <row r="146" spans="21:24">
-      <c r="U146" s="27"/>
-      <c r="V146" s="28"/>
-      <c r="W146" s="28"/>
-      <c r="X146" s="29"/>
+      <c r="U146" s="25"/>
+      <c r="V146" s="26"/>
+      <c r="W146" s="26"/>
+      <c r="X146" s="27"/>
     </row>
     <row r="147" spans="21:24">
-      <c r="U147" s="27"/>
-      <c r="V147" s="28"/>
-      <c r="W147" s="28"/>
-      <c r="X147" s="29"/>
+      <c r="U147" s="25"/>
+      <c r="V147" s="26"/>
+      <c r="W147" s="26"/>
+      <c r="X147" s="27"/>
     </row>
     <row r="148" spans="21:24">
-      <c r="U148" s="30"/>
-      <c r="V148" s="31"/>
-      <c r="W148" s="31"/>
-      <c r="X148" s="32"/>
+      <c r="U148" s="28"/>
+      <c r="V148" s="29"/>
+      <c r="W148" s="29"/>
+      <c r="X148" s="30"/>
     </row>
     <row r="237" spans="21:24">
-      <c r="U237" s="24" t="s">
+      <c r="U237" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="V237" s="25" t="s">
+      <c r="V237" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="W237" s="25" t="s">
+      <c r="W237" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="X237" s="25" t="s">
+      <c r="X237" s="23" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="238" spans="21:24">
-      <c r="U238" s="27" t="s">
+      <c r="U238" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="V238" s="28" t="s">
+      <c r="V238" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="W238" s="28" t="s">
+      <c r="W238" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="X238" s="28" t="s">
+      <c r="X238" s="26" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="239" spans="21:24">
-      <c r="U239" s="27"/>
-      <c r="V239" s="28"/>
-      <c r="W239" s="28"/>
-      <c r="X239" s="29"/>
+      <c r="U239" s="25"/>
+      <c r="V239" s="26"/>
+      <c r="W239" s="26"/>
+      <c r="X239" s="27"/>
     </row>
     <row r="240" spans="21:24">
-      <c r="U240" s="27"/>
-      <c r="V240" s="28"/>
-      <c r="W240" s="28"/>
-      <c r="X240" s="29"/>
+      <c r="U240" s="25"/>
+      <c r="V240" s="26"/>
+      <c r="W240" s="26"/>
+      <c r="X240" s="27"/>
     </row>
     <row r="241" spans="21:24">
-      <c r="U241" s="27"/>
-      <c r="V241" s="28"/>
-      <c r="W241" s="28"/>
-      <c r="X241" s="29"/>
+      <c r="U241" s="25"/>
+      <c r="V241" s="26"/>
+      <c r="W241" s="26"/>
+      <c r="X241" s="27"/>
     </row>
     <row r="242" spans="21:24">
-      <c r="U242" s="27"/>
-      <c r="V242" s="28"/>
-      <c r="W242" s="28"/>
-      <c r="X242" s="29"/>
+      <c r="U242" s="25"/>
+      <c r="V242" s="26"/>
+      <c r="W242" s="26"/>
+      <c r="X242" s="27"/>
     </row>
     <row r="243" spans="21:24">
-      <c r="U243" s="27"/>
-      <c r="V243" s="28"/>
-      <c r="W243" s="28"/>
-      <c r="X243" s="29"/>
+      <c r="U243" s="25"/>
+      <c r="V243" s="26"/>
+      <c r="W243" s="26"/>
+      <c r="X243" s="27"/>
     </row>
     <row r="244" spans="21:24">
-      <c r="U244" s="27"/>
-      <c r="V244" s="28"/>
-      <c r="W244" s="28"/>
-      <c r="X244" s="29"/>
+      <c r="U244" s="25"/>
+      <c r="V244" s="26"/>
+      <c r="W244" s="26"/>
+      <c r="X244" s="27"/>
     </row>
     <row r="245" spans="21:24">
-      <c r="U245" s="27"/>
-      <c r="V245" s="28"/>
-      <c r="W245" s="28"/>
-      <c r="X245" s="29"/>
+      <c r="U245" s="25"/>
+      <c r="V245" s="26"/>
+      <c r="W245" s="26"/>
+      <c r="X245" s="27"/>
     </row>
     <row r="246" spans="21:24">
-      <c r="U246" s="27"/>
-      <c r="V246" s="28"/>
-      <c r="W246" s="28"/>
-      <c r="X246" s="29"/>
+      <c r="U246" s="25"/>
+      <c r="V246" s="26"/>
+      <c r="W246" s="26"/>
+      <c r="X246" s="27"/>
     </row>
     <row r="247" spans="21:24">
-      <c r="U247" s="27"/>
-      <c r="V247" s="28"/>
-      <c r="W247" s="28"/>
-      <c r="X247" s="29"/>
+      <c r="U247" s="25"/>
+      <c r="V247" s="26"/>
+      <c r="W247" s="26"/>
+      <c r="X247" s="27"/>
     </row>
     <row r="248" spans="21:24">
-      <c r="U248" s="30"/>
-      <c r="V248" s="31"/>
-      <c r="W248" s="31"/>
-      <c r="X248" s="32"/>
+      <c r="U248" s="28"/>
+      <c r="V248" s="29"/>
+      <c r="W248" s="29"/>
+      <c r="X248" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30537,87 +31758,87 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:2">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="45">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="31" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="16.5">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="45" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="49" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="150">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="31" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="16.5">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="45" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="49" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="75">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="31" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="16.5">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="45" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="405">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="31" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="16.5">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="45" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="16.5">
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="46" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="45">
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="31" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="16.5">
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="47" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="45">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="31" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="48" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="255">
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="31" t="s">
         <v>154</v>
       </c>
     </row>
@@ -31166,24 +32387,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="57" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="2">
@@ -31313,7 +32534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143C98FA-68DF-475A-8166-946411EBDA91}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>

</xml_diff>